<commit_message>
added inline link to storage location on github
</commit_message>
<xml_diff>
--- a/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
+++ b/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>Comment</t>
   </si>
@@ -548,6 +548,12 @@
   </si>
   <si>
     <t>You need support? Drop a massage:</t>
+  </si>
+  <si>
+    <t>Template storage location:</t>
+  </si>
+  <si>
+    <t>https://github.com/nicolitschke/SysDevPm-templates/blob/master/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1644,6 +1650,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1661,12 +1673,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2001,7 +2007,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2017,58 +2023,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="98"/>
+      <c r="C2" s="100"/>
       <c r="D2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="98" t="s">
+      <c r="E2" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="99"/>
+      <c r="F2" s="101"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="100"/>
+      <c r="C3" s="102"/>
       <c r="D3" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="99"/>
+      <c r="F3" s="101"/>
     </row>
     <row r="4" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="96"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2407,6 +2413,14 @@
       <c r="F21" s="77" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D21)</f>
         <v>=D20&gt;D19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="94" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2463,9 +2477,10 @@
     <hyperlink ref="B26" r:id="rId1"/>
     <hyperlink ref="B24" r:id="rId2"/>
     <hyperlink ref="B25" r:id="rId3"/>
+    <hyperlink ref="B23" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2474,7 +2489,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2490,58 +2505,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="98"/>
+      <c r="C2" s="100"/>
       <c r="D2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="98" t="s">
+      <c r="E2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="99"/>
+      <c r="F2" s="101"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="100"/>
+      <c r="C3" s="102"/>
       <c r="D3" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="99"/>
+      <c r="F3" s="101"/>
     </row>
     <row r="4" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="96"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2790,6 +2805,14 @@
       <c r="F17" s="77" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D17)</f>
         <v>=D16&gt;D15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="94" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2847,8 +2870,9 @@
     <hyperlink ref="B22" r:id="rId1"/>
     <hyperlink ref="B20" r:id="rId2"/>
     <hyperlink ref="B21" r:id="rId3"/>
+    <hyperlink ref="B19" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the links to the toolbox-howto
Link to the toolbox-howto: https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Sch%C3%A4tzen.pdf?t=1600178241
Also typos updated
</commit_message>
<xml_diff>
--- a/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
+++ b/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Documents\Wissen\Templates\Safety\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
     <t>Comment</t>
   </si>
@@ -506,9 +506,6 @@
     <t>&lt;unique ID&gt;</t>
   </si>
   <si>
-    <t>Refer to »Guideline: Risiken quantifizieren«</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attribution-NonCommercial-ShareAlike 4.0 International (CC BY-NC-SA 4.0) </t>
   </si>
   <si>
@@ -553,7 +550,16 @@
     <t>Template storage location:</t>
   </si>
   <si>
-    <t>https://github.com/nicolitschke/SysDevPm-templates/blob/master/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx</t>
+    <t>HowTo</t>
+  </si>
+  <si>
+    <t>https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Sch%C3%A4tzen.pdf?t=1600178241</t>
+  </si>
+  <si>
+    <t>https://github.com/nicolitschke/SysDevPm-templates/raw/master/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx</t>
+  </si>
+  <si>
+    <t>Refer to »Toolbox: Produktfehler quantifizieren«</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -627,6 +633,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1392,7 +1405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1673,6 +1686,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2004,7 +2023,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2024,7 +2043,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="98"/>
@@ -2428,7 +2447,7 @@
         <v>70</v>
       </c>
       <c r="B24" s="94" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2441,12 +2460,20 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="93" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B26" s="94" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="B27" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2474,19 +2501,20 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1"/>
-    <hyperlink ref="B24" r:id="rId2"/>
-    <hyperlink ref="B25" r:id="rId3"/>
+    <hyperlink ref="B27" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId2"/>
+    <hyperlink ref="B26" r:id="rId3"/>
     <hyperlink ref="B23" r:id="rId4"/>
+    <hyperlink ref="B24" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2506,7 +2534,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="98"/>
@@ -2525,10 +2553,10 @@
       <c r="D2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="101"/>
+      <c r="E2" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="104"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
@@ -2820,9 +2848,8 @@
         <v>70</v>
       </c>
       <c r="B20" s="94" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="93"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="93" t="s">
@@ -2835,10 +2862,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="93" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B22" s="94" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="93"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="93" t="s">
         <v>64</v>
+      </c>
+      <c r="B23" s="94" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2867,12 +2903,14 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
-    <hyperlink ref="B21" r:id="rId3"/>
-    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B23" r:id="rId1"/>
+    <hyperlink ref="B21" r:id="rId2"/>
+    <hyperlink ref="B22" r:id="rId3"/>
+    <hyperlink ref="B20" r:id="rId4"/>
+    <hyperlink ref="B19" r:id="rId5"/>
+    <hyperlink ref="E2:F2" r:id="rId6" display="Refer to »Toolbox: Produktfehler quantifizieren«"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected hyperlink to the how-to
Link to how-to: https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Quantifizieren.pdf?t=1600416956
</commit_message>
<xml_diff>
--- a/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
+++ b/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
@@ -553,13 +553,13 @@
     <t>HowTo</t>
   </si>
   <si>
-    <t>https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Sch%C3%A4tzen.pdf?t=1600178241</t>
-  </si>
-  <si>
     <t>https://github.com/nicolitschke/SysDevPm-templates/raw/master/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx</t>
   </si>
   <si>
     <t>Refer to »Toolbox: Produktfehler quantifizieren«</t>
+  </si>
+  <si>
+    <t>https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Quantifizieren.pdf?t=1600416956</t>
   </si>
 </sst>
 </file>
@@ -1405,7 +1405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1693,6 +1693,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2026,7 +2027,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2434,12 +2435,12 @@
         <v>=D20&gt;D19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="93" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="93" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="94" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2447,7 +2448,7 @@
         <v>70</v>
       </c>
       <c r="B24" s="94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2517,7 +2518,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2554,7 +2555,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="103" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="104"/>
     </row>
@@ -2835,12 +2836,12 @@
         <v>=D16&gt;D15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="94" t="s">
-        <v>72</v>
+      <c r="B19" s="105" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2848,7 +2849,7 @@
         <v>70</v>
       </c>
       <c r="B20" s="94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2907,8 +2908,8 @@
     <hyperlink ref="B21" r:id="rId2"/>
     <hyperlink ref="B22" r:id="rId3"/>
     <hyperlink ref="B20" r:id="rId4"/>
-    <hyperlink ref="B19" r:id="rId5"/>
-    <hyperlink ref="E2:F2" r:id="rId6" display="Refer to »Toolbox: Produktfehler quantifizieren«"/>
+    <hyperlink ref="E2:F2" r:id="rId5" display="Refer to »Toolbox: Produktfehler quantifizieren«"/>
+    <hyperlink ref="B19" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
corrected hyperlink to how-to
link to how-to: https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Quantifizieren.pdf?t=1600416956
</commit_message>
<xml_diff>
--- a/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
+++ b/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
@@ -1405,7 +1405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1693,7 +1693,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2027,7 +2026,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2505,8 +2504,8 @@
     <hyperlink ref="B27" r:id="rId1"/>
     <hyperlink ref="B25" r:id="rId2"/>
     <hyperlink ref="B26" r:id="rId3"/>
-    <hyperlink ref="B23" r:id="rId4"/>
-    <hyperlink ref="B24" r:id="rId5"/>
+    <hyperlink ref="B24" r:id="rId4"/>
+    <hyperlink ref="B23" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2518,7 +2517,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2836,11 +2835,11 @@
         <v>=D16&gt;D15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="94" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor typos and license update
</commit_message>
<xml_diff>
--- a/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
+++ b/Safety-Management-Templates/Technical_Documents/TP_Safety_Failure_Risk_Estimation.xlsx
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>hrs</t>
   </si>
   <si>
@@ -506,9 +503,6 @@
     <t>&lt;unique ID&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Attribution-NonCommercial-ShareAlike 4.0 International (CC BY-NC-SA 4.0) </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Copyright </t>
     </r>
@@ -560,6 +554,12 @@
   </si>
   <si>
     <t>https://www.nicolitschke.com/app/download/8601498015/Toolbox_Produktfehler_Quantifizieren.pdf?t=1600416956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creative Commons Attribution-ShareAlike 4.0 International lizensiertl (CC BY-SA 4.0) </t>
+  </si>
+  <si>
+    <t>Assumptions</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0E53AE"/>
+        <fgColor rgb="FF64707D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1669,6 +1669,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1677,21 +1692,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1745,6 +1745,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF64707D"/>
       <color rgb="FF0E53AE"/>
       <color rgb="FF66FF66"/>
     </mruColors>
@@ -2025,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2042,53 +2043,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="A1" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="104"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="100"/>
+        <v>49</v>
+      </c>
+      <c r="B2" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="97"/>
       <c r="D2" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="100" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="101"/>
+        <v>53</v>
+      </c>
+      <c r="E2" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="98"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="102" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="101"/>
+      <c r="E3" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="95"/>
       <c r="D4" s="95"/>
@@ -2099,30 +2100,30 @@
     <row r="6" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="82"/>
       <c r="B6" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="83" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="84" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="84" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="80" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="90">
         <v>15</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
@@ -2130,20 +2131,20 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="91">
         <v>8000</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="92">
         <f>B8/B7</f>
         <v>533.33333333333337</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="66" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D8)</f>
@@ -2152,20 +2153,20 @@
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="21">
         <f>SUM(D10:D15)</f>
         <v>3.8125100000000002E-2</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="85" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D9)</f>
@@ -2174,20 +2175,20 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="23">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3">
         <f>B10/B8</f>
         <v>6.2500000000000001E-4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="60" t="str">
         <f t="shared" ref="F10:F17" ca="1" si="0">_xlfn.FORMULATEXT(D10)</f>
@@ -2196,20 +2197,20 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="23">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
         <f>B11/D8</f>
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="60" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2218,20 +2219,20 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="23">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <f>B12/D8</f>
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="60" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2240,20 +2241,20 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="23">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1">
         <f>B13/D8</f>
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="60" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2262,20 +2263,20 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="23">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="4">
         <f>B14/D8</f>
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="60" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2284,20 +2285,20 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="28">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5">
         <f>B15</f>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="87" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2306,20 +2307,20 @@
     </row>
     <row r="16" spans="1:6" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A16" s="63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="25">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="11">
         <f>B16</f>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="64" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2328,13 +2329,13 @@
     </row>
     <row r="17" spans="1:6" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A17" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="41">
         <v>0.2</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="42">
         <f>B17</f>
@@ -2348,20 +2349,20 @@
     </row>
     <row r="18" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="88" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="29">
         <v>0.1</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="31">
         <f>B18/3600</f>
         <v>2.7777777777777779E-5</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="89" t="str">
         <f t="shared" ref="F18" ca="1" si="1">_xlfn.FORMULATEXT(D18)</f>
@@ -2370,20 +2371,20 @@
     </row>
     <row r="19" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="38">
         <f>D9*D16*D17*D18</f>
         <v>2.1180611111111114E-14</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="69" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D19)</f>
@@ -2392,20 +2393,20 @@
     </row>
     <row r="20" spans="1:6" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="40">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="34">
         <f>B20</f>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="71" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D20)</f>
@@ -2414,20 +2415,20 @@
     </row>
     <row r="21" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="75" t="b">
         <f>D20&gt;D19</f>
         <v>1</v>
       </c>
       <c r="E21" s="76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="77" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D21)</f>
@@ -2436,42 +2437,42 @@
     </row>
     <row r="23" spans="1:6" s="93" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="94" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="94" t="s">
         <v>70</v>
-      </c>
-      <c r="B24" s="94" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="93" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B25" s="94" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="93" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26" s="94" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="93" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" s="94" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D27" s="10"/>
     </row>
@@ -2501,11 +2502,11 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B27" r:id="rId1"/>
-    <hyperlink ref="B25" r:id="rId2"/>
-    <hyperlink ref="B26" r:id="rId3"/>
-    <hyperlink ref="B24" r:id="rId4"/>
-    <hyperlink ref="B23" r:id="rId5"/>
+    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B26" r:id="rId2"/>
+    <hyperlink ref="B24" r:id="rId3"/>
+    <hyperlink ref="B23" r:id="rId4"/>
+    <hyperlink ref="B27" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -2517,7 +2518,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2533,53 +2534,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="A1" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="104"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="100" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="100"/>
+        <v>49</v>
+      </c>
+      <c r="B2" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="97"/>
       <c r="D2" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="103" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="104"/>
+        <v>53</v>
+      </c>
+      <c r="E2" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="101"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="102" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="102"/>
+      <c r="C3" s="99"/>
       <c r="D3" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="100" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="101"/>
+      <c r="F3" s="98"/>
     </row>
     <row r="4" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="95"/>
       <c r="D4" s="95"/>
@@ -2590,30 +2591,30 @@
     <row r="6" spans="1:6" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="54" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="54" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="80" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="78">
         <v>15</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
@@ -2621,20 +2622,20 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="79">
         <v>6000</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="51">
         <f>B8/B7</f>
         <v>400</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="56" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D8)</f>
@@ -2643,20 +2644,20 @@
     </row>
     <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="48">
         <f>SUM(D10:D11)</f>
         <v>3.7500000000000006E-2</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="58" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D9)</f>
@@ -2665,20 +2666,20 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="23">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1">
         <f>B10/D8</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="60" t="str">
         <f t="shared" ref="F10:F14" ca="1" si="0">_xlfn.FORMULATEXT(D10)</f>
@@ -2687,20 +2688,20 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="24">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="20">
         <f>B11/D8</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="62" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2709,20 +2710,20 @@
     </row>
     <row r="12" spans="1:6" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A12" s="63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="11">
         <f>B12</f>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="64" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2731,20 +2732,20 @@
     </row>
     <row r="13" spans="1:6" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A13" s="65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="26">
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="15">
         <f>B13</f>
         <v>1</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="66" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2753,20 +2754,20 @@
     </row>
     <row r="14" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="27">
         <v>0.06</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="18">
         <f>B14/3600*24/60*1000/(365*24)</f>
         <v>7.6103500761035006E-7</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="56" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2775,20 +2776,20 @@
     </row>
     <row r="15" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="38">
         <f>D9*D12*D13*D14</f>
         <v>2.8538812785388128E-14</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="69" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D15)</f>
@@ -2797,20 +2798,20 @@
     </row>
     <row r="16" spans="1:6" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="40">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="34">
         <f>B16</f>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="71" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D16)</f>
@@ -2819,11 +2820,11 @@
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="73"/>
       <c r="C17" s="74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="75" t="b">
         <f>D16&gt;D15</f>
@@ -2837,44 +2838,44 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="94" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="94" t="s">
         <v>70</v>
-      </c>
-      <c r="B20" s="94" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="93" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="94" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="93"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="93" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="94" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="93"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="93" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="94" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2903,12 +2904,12 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B23" r:id="rId1"/>
-    <hyperlink ref="B21" r:id="rId2"/>
-    <hyperlink ref="B22" r:id="rId3"/>
-    <hyperlink ref="B20" r:id="rId4"/>
-    <hyperlink ref="E2:F2" r:id="rId5" display="Refer to »Toolbox: Produktfehler quantifizieren«"/>
-    <hyperlink ref="B19" r:id="rId6"/>
+    <hyperlink ref="B21" r:id="rId1"/>
+    <hyperlink ref="B22" r:id="rId2"/>
+    <hyperlink ref="B20" r:id="rId3"/>
+    <hyperlink ref="E2:F2" r:id="rId4" display="Refer to »Toolbox: Produktfehler quantifizieren«"/>
+    <hyperlink ref="B19" r:id="rId5"/>
+    <hyperlink ref="B23" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>